<commit_message>
move to js proto
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="static_table_1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
     <t>desc</t>
   </si>
   <si>
-    <t>static_table_1_id</t>
+    <t>static_table_1_refid</t>
   </si>
 </sst>
 </file>
@@ -376,8 +376,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:C2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -486,8 +486,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>